<commit_message>
comments, authors, and time
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,16 @@
           <t>Comments</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Authors</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Dates</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -449,6 +459,16 @@
           <t>山科智能长箭射天之否定</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>美妙歌声</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>09-13 04:21</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -459,6 +479,16 @@
           <t>超短波段实盘</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>chaoshou22</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>08-31 05:58</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -469,6 +499,16 @@
           <t>了结金科，收下15CM，缩量震荡，个股性行情！</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>摆渡人88</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>08-30 04:01</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -479,6 +519,16 @@
           <t>8.30首先感谢朋友们的关心，老人身体无大碍，但仍要住院治疗几天。在医院流风只能</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>流风回血</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>08-30 03:29</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -489,6 +539,16 @@
           <t>超短波段实盘</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>chaoshou22</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>08-30 09:51</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -499,6 +559,16 @@
           <t>$山科智能(有人问我股票能炒吗，我跟他说，什么兴趣爱好都可以，哪怕你天天打游戏，</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>奥力给888</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>08-30 07:38</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -509,6 +579,16 @@
           <t>金科股份强势封板！皆大欢喜！普天同庆！</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>摆渡人88</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>08-29 03:40</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -519,6 +599,16 @@
           <t>8.29上午老人因交通事故致伤被肇事方送往医院，本人接到电话也第一时间赶到，还好</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>流风回血</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>08-29 08:04</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -529,6 +619,16 @@
           <t>20230829（周二 收盘）</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>股海小歧</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>08-29 07:43</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -539,6 +639,16 @@
           <t>20230828（周一 收盘）</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>股海小歧</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>08-28 10:50</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -549,6 +659,16 @@
           <t>污水处理概念：一直被低估！未来有望主升可能的行业龙头</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>我想找个男朋友</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>08-26 02:12</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -559,6 +679,16 @@
           <t>以全流程服务体系领引智慧水务新方向  山科智能2023年半年度营业收入同比增长33.69%</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>全景网</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>08-22 04:42</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -569,6 +699,16 @@
           <t>山科智能中报出炉：业绩增长但现金流量净额亏损，财务状况引发关注【BT财报快闪】</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>BT财经</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>08-22 03:00</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -579,6 +719,16 @@
           <t>，：</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>股友0R087A9259</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>08-16 10:00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -589,6 +739,16 @@
           <t>：：</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>股友0R087A9259</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>08-16 09:39</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -599,6 +759,16 @@
           <t>：：</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>股友0R087A9259</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>08-15 01:13</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -609,6 +779,16 @@
           <t>山科智能(300897.SZ)发布上半年业绩，净利润3682万元，同比增长18.23%</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>智通财经</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>08-14 06:30</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -619,6 +799,16 @@
           <t>中国星链计划-国安军工，漫漫涨停开启</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>托塔金天王</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>08-03 05:50</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -629,6 +819,16 @@
           <t>十优打板：国芳集团（SH601086）缠论技术分析</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>十优缠论</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>07-31 08:27</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -639,6 +839,16 @@
           <t>山科智能300897长短期均线“粘合顺上↑”看多跟踪。</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>祥云0303</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>07-30 12:16</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -649,6 +859,16 @@
           <t>下星期指数看3335---3350，下星期一是月线收盘，券商指数是月线反转，上证指数是周线月线趋势反转点共振，期待银行复制券商</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GUyou868C06F186</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>07-28 11:11</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -659,6 +879,16 @@
           <t>说了关注股票软件相关个股，说了财富趋势同花顺大智慧金证股份今天全都是涨停。东方财富11%，首创证券太平洋信达证券天风证券都是涨停</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GUyou10K3531K59</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>07-28 10:36</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -669,6 +899,16 @@
           <t>25号直播间还特意说了券商加仓的最好机会是本周星期四或者星期五，今天券商大面积涨停，指数上涨7.42%，下一个看好券商银行</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GU181A7006B9948</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>07-28 10:26</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -679,6 +919,16 @@
           <t>分享688667，机会自己把握</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>白云黄鹤</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>07-21 10:10</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -689,6 +939,16 @@
           <t>山科智能(300897.SZ):数字孪生平台从6月份开始意向客户明显增多</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>格隆汇</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>07-13 06:15</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -699,6 +959,16 @@
           <t>山科智能(300897.SZ):“年产200万套智能传感器项目”一期已于2021年投入使用</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>格隆汇</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>07-13 06:15</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -709,6 +979,16 @@
           <t>山科智能(300897.SZ):目前公司90%以上的客户为自来水公司</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>格隆汇</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>07-13 06:14</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -719,6 +999,16 @@
           <t>山科智能(300897.SZ):公司二季度经营情况一切正常</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>格隆汇</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>07-13 06:14</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -729,6 +1019,16 @@
           <t>山科智能(300897.SZ):将继续进一步发展智慧水利作为公司战略规划之一</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>格隆汇</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>07-13 06:10</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -739,6 +1039,16 @@
           <t>山科智能300897长短期均线“粘合顺上↑”看多跟踪。</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>祥云0303</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>06-27 09:04</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -749,6 +1059,16 @@
           <t>水表比电表还是要差蛮多的。。。</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>函股论道</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>06-15 08:38</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -759,6 +1079,16 @@
           <t>还是低吸，等待</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>小散的成长路</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>06-06 07:29</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -769,6 +1099,16 @@
           <t>山科/数字中国_4股：AⅠ算力与人工智能明日之光芒璀璨</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>论股浅水</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>06-05 06:20</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -779,6 +1119,16 @@
           <t>山科智能300897长短期均线“粘合顺上↑”看多跟踪。</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>祥云0303</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>06-02 10:05</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -789,6 +1139,16 @@
           <t>山科智能</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>股友10g83135g7</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>05-31 01:26</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -799,6 +1159,16 @@
           <t>短线有调整，未来预期还是看好。。。</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>函股论道</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>05-30 11:31</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -809,6 +1179,16 @@
           <t>太垃圾了</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>有魅力之霹雳火</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>05-30 09:55</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -819,6 +1199,16 @@
           <t>套牢在40以上筹码太多了，不磨走这些筹码，主力是不会当雷F来抬轿为他们解套的。。这就需要时间。。</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>函股论道</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>05-30 12:49</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -829,6 +1219,16 @@
           <t>【300897山科智能】红牛一定能够赚钱出场的，而且就是明天，这就是技术！操作！</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>账户已注销</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>05-29 09:57</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -839,6 +1239,16 @@
           <t>分红明天到账吗</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>李百万1</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>05-29 03:02</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -849,6 +1259,16 @@
           <t>小盘股还有振荡反弹的机会，36计比谁跑的快</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>股势仁升</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>05-29 04:36</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -859,6 +1279,16 @@
           <t>11连板开始了，10万到100万第46天记录,24万，已经翻倍。</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>小懒财富日记</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>05-26 06:39</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -869,6 +1299,16 @@
           <t>山科日线上应会有调整，周线应还有机会。</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>函股论道</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>05-26 07:23</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -879,6 +1319,16 @@
           <t>山科智能：AI+国家水网+智能机器人+华为+杭州</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>股友8229A1</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>05-26 10:47</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -889,6 +1339,16 @@
           <t>山科智能2022年度业绩说明会于2023年4月26日（星期三）下午15:00-1</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>李百万1</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>05-25 10:12</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -899,6 +1359,16 @@
           <t>5.25早评指数见底明朗，需要耐心等待</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>腾飞老马</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>05-25 08:24</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -909,6 +1379,16 @@
           <t>中共中央、国务院印发了《国家水网建设规划纲要》，并发出通知，要求各地区各部门结合</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>宝宝铁粉</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>05-25 08:27</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -919,6 +1399,16 @@
           <t>中期看好，票是好票，短期有回调。。</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>函股论道</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>05-25 05:06</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -929,6 +1419,16 @@
           <t>5.24叠加中特估跳空低开，盘中形成新低？</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>流浪股民77</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>05-24 05:14</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -939,6 +1439,16 @@
           <t>市场“智能”成瘾症？ 不是人工智能的山科智能最高涨超17%</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>看究竟app</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>05-24 04:18</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -949,6 +1459,16 @@
           <t>明天周三，有机会低吸的5只翻倍趋势黑马，值得关注验证！1、山科智能300897最</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>财经小花姐</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>05-23 07:21</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -959,6 +1479,16 @@
           <t>山科智能2022年度业绩说明会【全景路演】</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>山科智能</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>04-20 11:28</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -969,6 +1499,16 @@
           <t>山科智能(300897.SZ)中标2277.8万元户用远传水表采购及安装项目</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>智通财经</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>03-27 06:18</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -979,6 +1519,16 @@
           <t>山科智能300897长短期均线“粘合顺上↑”看多跟踪。</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>祥云0303</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>03-28 12:07</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -989,6 +1539,16 @@
           <t>山科可以加智能机器智慧城市和国产软件</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>广888888发</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>03-01 11:57</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -999,6 +1559,16 @@
           <t>智能水表行业发展趋势预测：需求规模持续扩张，市场竞争愈发激烈</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>智研咨询</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>02-27 10:02</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1009,6 +1579,16 @@
           <t>年报期间，潜伏绩优股山科智能，去年一季度业绩一毛三，二季度4毛，去年三季度7毛3</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>番茄小号</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>01-13 02:33</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1019,6 +1599,16 @@
           <t>股价破发超8个月，山科智能大股东减持时间过半未减持</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>泡财经APP</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>11-02 06:46</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1029,6 +1619,16 @@
           <t>写字楼招商|山科智能大厦，信息化智慧办公环境期待您的入驻山科智能2022-01-</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>哈哈哈哈哈哈711</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>08-27 02:29</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1039,6 +1639,16 @@
           <t>智慧水务产品获认可 山科智能中标3078万元NB-IoT户用远传水表项目</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>大吉为富de火舞你</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>08-16 06:50</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1049,6 +1659,16 @@
           <t>磁悬浮制冷压缩机概念股</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>大海微蓝</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>07-21 11:40</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1059,6 +1679,16 @@
           <t>情绪冰点转折开始新的一轮。底部个股上涨的开始</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>老金天下</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>07-21 08:58</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1069,6 +1699,16 @@
           <t>$山科智能(SZ300897)$山科今天的走势不错极好:第一阳包阴，扭转了跌的态</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>A财神到A</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>06-10 09:30</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1079,6 +1719,16 @@
           <t>利好消息！</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>大司马论市</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>05-17 10:50</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1089,6 +1739,16 @@
           <t>北上资金、杠杆资金逆势加仓9只绩优股</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>指数增强小霸王</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>04-29 12:24</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1099,6 +1759,16 @@
           <t>山科智能2021年度业绩说明会【全景路演】</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>山科智能</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>04-23 12:15</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1109,6 +1779,16 @@
           <t>山科可能又不送股</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>稳操胜券bqn8jr</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>04-18 08:57</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1119,6 +1799,16 @@
           <t>年报如不十送十,后果很严重.</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>高尔础</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>02-16 09:41</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1129,6 +1819,16 @@
           <t>知情达理雪梨ZN：老师预测一下山科智能后期走势可以吗，谢谢山科智能2021.7.</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>蔚蓝大海A</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>10-25 04:38</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1139,6 +1839,16 @@
           <t>8日，水务股早盘集体走高，重庆水务、钱江水利、绿城水务、江南水务等涨停。消息面上</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>guy1234</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>10-08 10:28</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1149,6 +1859,16 @@
           <t>资讯：6日，水务股早盘集体走高，北控水务集团(00371)涨12.01%，报3.</t>
         </is>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>guy1234</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>10-07 07:21</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1159,6 +1879,16 @@
           <t>底部了缩量快9个月，还差一个点火题材，可惜假期鲜有人吹智慧水网，只有在电网与其他</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>kk11000</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>10-05 11:48</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1169,6 +1899,16 @@
           <t>300897山科智能。2020.10.28创下新高后，股价一路向下，一泻千里，几</t>
         </is>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>蔚蓝大海A</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>08-10 07:24</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1179,6 +1919,16 @@
           <t>上市公司这样做让所有股民嗨了！第一目标50元！如此重大利好竟被视而不见！只要捐款</t>
         </is>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>你是股神123456</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>07-31 07:35</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1187,6 +1937,16 @@
       <c r="B76" t="inlineStr">
         <is>
           <t>公司董事会：希望公司能倾听建设性建议，送股是提升市值的必要途经。以4月19日为例</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>喝茶喝茶</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>04-24 05:21</t>
         </is>
       </c>
     </row>

</xml_diff>